<commit_message>
Old HMI desing using touchgfx
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="1"/>
   <bookViews>
-    <workbookView windowWidth="16380" windowHeight="8190"/>
+    <workbookView windowWidth="16380" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
-    <sheet name="Translation" sheetId="2" r:id="rId2"/>
+    <sheet name="Translation" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
+  <calcPr calcId="145621" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -26,158 +26,128 @@
     <t xml:space="preserve">Bpp</t>
   </si>
   <si>
+    <t xml:space="preserve">TouchGFX - Typography Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TouchGFX - Translation Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildcard Ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallback Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pixel size of the font as an integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bit depth of the font. Valid values are 1, 2, 4 and 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The character to write if a glyph is missing at runtime (blank causes assert if glyph is missing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The characters that are used in wildcard strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to "Wildcard Characters", but can be used to easily specify a range of characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48-57,65-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x30-0x39,0x41-0x48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For more information read about "Using texts and fonts" on http://support.touchgfx.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellipsis Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The character to insert when truncating long lines. See TextArea::setWideTextAction()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPOGRAPHY NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">GB</t>
   </si>
   <si>
-    <t xml:space="preserve">TouchGFX - Typography Sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TouchGFX - Translation Sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typography Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add additional language columns here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DigitalClock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;time&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital_clock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asap-Regular.ttf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fallback Character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wildcard Characters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wildcard Ranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APM :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The pixel size of the font as an integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The bit depth of the font. Valid values are 1, 2, 4 and 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The character to write if a glyph is missing at runtime (blank causes assert if glyph is missing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The characters that are used in wildcard strings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567890.-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Similar to "Wildcard Characters", but can be used to easily specify a range of characters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-9,A-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48-57,65-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x30-0x39,0x41-0x48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For more information read about "Using texts and fonts" on http://support.touchgfx.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ellipsis Character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The character to insert when truncating long lines. See TextArea::setWideTextAction()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x22EF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEXT ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPOGRAPHY NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALIGNMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD ADDITIONAL LANGUAGE HERE (1 TO 3 CAPITAL LETTERS) - 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD ADDITIONAL LANGUAGE HERE (1 TO 3 CAPITAL LETTERS) - 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD ADDITIONAL LANGUAGE HERE (1 TO 3 CAPITAL LETTERS) - 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right</t>
-  </si>
-  <si>
     <t xml:space="preserve">Widget Wildcard Characters</t>
   </si>
   <si>
-    <t xml:space="preserve">0123456789 :APM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIRECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdana.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -220,13 +190,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -236,8 +200,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,8 +229,19 @@
         <bgColor rgb="FF4F81BD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -261,117 +251,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -383,19 +262,163 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -477,56 +500,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="82">
+    <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1"/>
     <cellStyle name="Normal 10 2" xfId="2"/>
@@ -609,23 +628,7 @@
     <cellStyle name="Normal 8" xfId="79"/>
     <cellStyle name="Normal 9" xfId="80"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -864,13 +867,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="secondRowStripe" dxfId="13"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="firstColumn" dxfId="15"/>
+      <tableStyleElement type="lastColumn" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="11"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -885,7 +888,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
   <sortState ref="B4:E6">
     <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
@@ -905,30 +908,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" dataDxfId="5"/>
-    <tableColumn id="2" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" name="Example 1" dataDxfId="3"/>
-    <tableColumn id="4" name="Example 2" dataDxfId="2"/>
-    <tableColumn id="5" name="Example 3" dataDxfId="1"/>
+    <tableColumn id="1" name="Column" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
+    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
+    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:H800" totalsRowShown="0" tableBorderDxfId="0">
-  <tableColumns count="7">
-    <tableColumn id="1" name="Text ID"/>
-    <tableColumn id="2" name="Typography Name"/>
-    <tableColumn id="3" name="Alignment"/>
-    <tableColumn id="4" name="GB"/>
-    <tableColumn id="6" name="Add additional language here (1 to 3 capital letters) - 2"/>
-    <tableColumn id="7" name="Add additional language here (1 to 3 capital letters) - 3"/>
-    <tableColumn id="8" name="Add additional language here (1 to 3 capital letters) - 4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1306,22 +1294,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0.28515625" style="0" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="0" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="0" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" style="0" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" style="0" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="0" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" style="0" customWidth="1"/>
     <col min="12" max="12" width="20.140625" style="0" customWidth="1"/>
     <col min="13" max="13" width="84.7109375" style="0" bestFit="1" customWidth="1"/>
@@ -1337,199 +1325,221 @@
       <c r="E1"/>
     </row>
     <row r="2" spans="2:16" ht="39.95" customHeight="1" thickBot="1">
-      <c r="B2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>36</v>
+      <c r="J3" s="20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4"/>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
       <c r="J4"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>21</v>
+      <c r="L4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="K5" s="3"/>
-      <c r="L5" s="8" t="s">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="L5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="10">
+      <c r="M5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="9">
         <v>20</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>36</v>
       </c>
-      <c r="P5" s="11"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="K6" s="3"/>
-      <c r="L6" s="8" t="s">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="L6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="10">
+      <c r="M6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="9">
         <v>4</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>8</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="K7" s="3"/>
-      <c r="L7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>27</v>
+      <c r="L7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:16">
-      <c r="K8" s="3"/>
-      <c r="L8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="11"/>
+      <c r="L8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
-      <c r="K9" s="3"/>
-      <c r="L9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="P9" s="15" t="s">
-        <v>34</v>
+      <c r="L9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:16">
-      <c r="K10" s="3"/>
-      <c r="L10" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="22"/>
+      <c r="L10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="K11" s="3"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="M12" s="21" t="s">
-        <v>35</v>
+      <c r="M12" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1549,89 +1559,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I5"/>
+  <dimension ref="B1:F3"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" style="0" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.42578125" style="0" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="0" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="0" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="0" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="0" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="129" hidden="1" customHeight="1">
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
+    <row r="1" spans="2:6" ht="3.75" customHeight="1"/>
+    <row r="2" spans="2:6" ht="33" customHeight="1">
+      <c r="B2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
-    <row r="2" spans="2:9" ht="39.95" customHeight="1">
-      <c r="B2" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="3" t="s">
-        <v>7</v>
+    <row r="3" spans="2:6" s="22" customFormat="1">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="15" customHeight="1">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" s="3" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added needle for speedometer
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,30 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">99999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
   </si>
 </sst>
 </file>
@@ -1601,6 +1625,23 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Use 2 custom touchgfx font
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="56">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
   </si>
 </sst>
 </file>
@@ -1675,7 +1678,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Change text to wildcard
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="59">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
   </si>
 </sst>
 </file>
@@ -1426,7 +1435,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1686,13 +1697,30 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added initial value to new text
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="60">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1691,40 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added new touchgfx design
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,60 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">99999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB-DIRECTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB-ALIGNMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB-TYPOGRAPHY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResourceId1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;value&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00000</t>
   </si>
 </sst>
 </file>
@@ -1438,9 +1384,7 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4" t="s">
-        <v>56</v>
-      </c>
+      <c r="I4"/>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1657,74 +1601,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Separate the background image
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1621,40 +1621,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="4"/>
+    <row r="5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Change font single to resource
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="59">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1433,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1463,7 +1471,9 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
@@ -1648,7 +1658,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -1663,23 +1673,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="6"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
New container for background
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="75">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -192,6 +192,54 @@
   </si>
   <si>
     <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECONOMIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIP A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">888 KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88.8 KM/KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERSONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
   </si>
 </sst>
 </file>
@@ -1492,6 +1540,23 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1673,7 +1738,159 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added scroll wheel for drive mode
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="94">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t xml:space="preserve">%/ RANGEVKMWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1784,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1795,13 +1801,13 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -1812,7 +1818,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -1829,10 +1835,10 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -1846,13 +1852,13 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -1863,13 +1869,13 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
@@ -1880,24 +1886,24 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -1914,10 +1920,10 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
@@ -1926,15 +1932,15 @@
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>
@@ -1943,12 +1949,12 @@
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
@@ -1965,10 +1971,10 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
         <v>51</v>
@@ -1977,15 +1983,15 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>51</v>
@@ -1994,15 +2000,15 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
         <v>51</v>
@@ -2011,32 +2017,32 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -2045,9 +2051,11 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
-      </c>
-    </row>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Handling report mode container
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="104">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -297,6 +297,36 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM</t>
   </si>
 </sst>
 </file>
@@ -1835,24 +1865,24 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -1864,29 +1894,29 @@
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -1898,12 +1928,12 @@
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -1915,32 +1945,32 @@
         <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>
@@ -1949,29 +1979,29 @@
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -1988,7 +2018,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -2000,12 +2030,12 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -2017,18 +2047,18 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
@@ -2039,10 +2069,10 @@
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -2051,11 +2081,43 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21"/>
-    <row r="22"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Fix LCD flicker by reduce LTDC clock freq.
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4132" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4486" uniqueCount="124">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPS: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
   </si>
 </sst>
 </file>
@@ -2271,6 +2280,40 @@
         <v>100</v>
       </c>
     </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added more debug parameters
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4678" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5566" uniqueCount="138">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -396,6 +396,39 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2370,7 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
@@ -2357,6 +2390,92 @@
         <v>90</v>
       </c>
     </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added dedicated fingerprint response icon
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5566" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5782" uniqueCount="138">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2458,23 +2458,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37">
-      <c r="B37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" t="s">
-        <v>137</v>
-      </c>
-    </row>
+    <row r="37"/>
     <row r="38"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Refactor & add CAN connection status
</commit_message>
<xml_diff>
--- a/HMI-APP/TouchGFX/assets/texts/texts.xlsx
+++ b/HMI-APP/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5782" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6616" uniqueCount="139">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN DISCONNECTED</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2327,7 @@
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -2336,12 +2339,12 @@
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
@@ -2358,7 +2361,7 @@
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
         <v>44</v>
@@ -2370,12 +2373,12 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
@@ -2392,7 +2395,7 @@
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -2404,12 +2407,12 @@
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -2426,10 +2429,10 @@
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
         <v>51</v>
@@ -2438,26 +2441,10 @@
         <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" t="s">
-        <v>90</v>
-      </c>
-    </row>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36"/>
     <row r="37"/>
     <row r="38"/>
   </sheetData>

</xml_diff>